<commit_message>
Modify power of L4
</commit_message>
<xml_diff>
--- a/OperateString/TestDefGeneration/TX_RF_FUNC/Pamukkale_R1B_Regression.xlsx
+++ b/OperateString/TestDefGeneration/TX_RF_FUNC/Pamukkale_R1B_Regression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RuPyTest_P1A03\OperateString\TestDefGeneration\TX_RF_FUNC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C954EC9-DC4E-4A42-90FE-11250496AC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA517CF3-EDB9-4EA6-A228-4AB0488BA3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CarrierLimit" sheetId="1" r:id="rId1"/>
@@ -283,9 +283,6 @@
     <t>testDef_head</t>
   </si>
   <si>
-    <t>C:\RuxTest_R9J\TestDefs\_RRU4417_B1_head.txt</t>
-  </si>
-  <si>
     <t>output_file_name</t>
   </si>
   <si>
@@ -985,6 +982,10 @@
   </si>
   <si>
     <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\RuxTest_R9J\TestDefs\_RRU4417_B1_head.txt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3469,7 +3470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -3477,10 +3478,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3545,30 +3546,30 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F5" t="s">
+        <v>278</v>
+      </c>
+      <c r="G5" t="s">
         <v>134</v>
-      </c>
-      <c r="C5" t="s">
-        <v>276</v>
-      </c>
-      <c r="D5" t="s">
-        <v>277</v>
-      </c>
-      <c r="E5" t="s">
-        <v>278</v>
-      </c>
-      <c r="F5" t="s">
-        <v>279</v>
-      </c>
-      <c r="G5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -3633,30 +3634,30 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" t="s">
+        <v>280</v>
+      </c>
+      <c r="D11" t="s">
         <v>281</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>282</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>283</v>
       </c>
-      <c r="F11" t="s">
-        <v>284</v>
-      </c>
       <c r="G11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -3721,30 +3722,30 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s">
+        <v>286</v>
+      </c>
+      <c r="D17" t="s">
         <v>287</v>
       </c>
-      <c r="D17" t="s">
-        <v>288</v>
-      </c>
       <c r="E17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -3809,30 +3810,30 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s">
+        <v>293</v>
+      </c>
+      <c r="D23" t="s">
         <v>294</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>295</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>296</v>
       </c>
-      <c r="F23" t="s">
-        <v>297</v>
-      </c>
       <c r="G23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -3897,30 +3898,30 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C29" t="s">
+        <v>289</v>
+      </c>
+      <c r="D29" t="s">
         <v>290</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>292</v>
+      </c>
+      <c r="F29" t="s">
         <v>291</v>
       </c>
-      <c r="E29" t="s">
-        <v>293</v>
-      </c>
-      <c r="F29" t="s">
-        <v>292</v>
-      </c>
       <c r="G29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -3985,30 +3986,30 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C35" t="s">
+        <v>301</v>
+      </c>
+      <c r="D35" t="s">
         <v>302</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>303</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>304</v>
       </c>
-      <c r="F35" t="s">
-        <v>305</v>
-      </c>
       <c r="G35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -4073,30 +4074,30 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C41" t="s">
+        <v>305</v>
+      </c>
+      <c r="D41" t="s">
         <v>306</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>307</v>
       </c>
-      <c r="E41" t="s">
-        <v>308</v>
-      </c>
       <c r="F41" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -4161,22 +4162,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C47" t="s">
+        <v>310</v>
+      </c>
+      <c r="D47" t="s">
+        <v>312</v>
+      </c>
+      <c r="E47" t="s">
         <v>311</v>
       </c>
-      <c r="D47" t="s">
-        <v>313</v>
-      </c>
-      <c r="E47" t="s">
-        <v>312</v>
-      </c>
       <c r="F47" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4216,7 +4217,7 @@
         <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>51</v>
@@ -4227,7 +4228,7 @@
         <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -4236,7 +4237,7 @@
         <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -4344,7 +4345,7 @@
         <v>66</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -4503,8 +4504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4532,67 +4533,67 @@
         <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -4620,7 +4621,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" s="2">
         <v>2110</v>
@@ -4628,7 +4629,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="2">
         <v>2170</v>
@@ -4636,23 +4637,23 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>50</v>
@@ -4660,10 +4661,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -4671,19 +4672,19 @@
         <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -4691,7 +4692,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
@@ -4711,7 +4712,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>21</v>
@@ -4863,10 +4864,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
         <v>113</v>
-      </c>
-      <c r="B1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4886,25 +4887,25 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -4924,25 +4925,25 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -4962,25 +4963,25 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -5000,25 +5001,25 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -5038,25 +5039,25 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -5076,25 +5077,25 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -5114,25 +5115,25 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -5152,17 +5153,17 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -5183,10 +5184,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -5215,18 +5216,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
         <v>134</v>
-      </c>
-      <c r="C5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -5255,18 +5256,18 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -5295,18 +5296,18 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -5335,18 +5336,18 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -5375,18 +5376,18 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -5415,18 +5416,18 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -5455,18 +5456,18 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -5495,18 +5496,18 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -5535,18 +5536,18 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -5575,18 +5576,18 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C59" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B61" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -5615,18 +5616,18 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B67" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -5655,18 +5656,18 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C71" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B73" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -5695,18 +5696,18 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C77" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B79" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -5735,18 +5736,18 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C83" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B85" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -5775,18 +5776,18 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C89" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B91" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -5815,18 +5816,18 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C95" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B97" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -5855,18 +5856,18 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C101" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B103" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -5895,18 +5896,18 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C107" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B109" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -5935,18 +5936,18 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C113" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -5975,18 +5976,18 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C119" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B121" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -6015,18 +6016,18 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C125" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B127" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -6055,18 +6056,18 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C131" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B133" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -6095,18 +6096,18 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C137" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B139" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -6135,18 +6136,18 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C143" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B145" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
@@ -6175,18 +6176,18 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C149" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B151" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -6215,18 +6216,18 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C155" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
@@ -6255,18 +6256,18 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C161" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B163" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
@@ -6295,18 +6296,18 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C167" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B169" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
@@ -6335,18 +6336,18 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C173" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B175" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
@@ -6375,18 +6376,18 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C179" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B181" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
@@ -6415,18 +6416,18 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C185" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B187" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
@@ -6455,18 +6456,18 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C191" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B193" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
@@ -6495,18 +6496,18 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C197" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B199" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
@@ -6535,18 +6536,18 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C203" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B205" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
@@ -6575,18 +6576,18 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B209" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C209" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B211" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
@@ -6615,10 +6616,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B215" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C215" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -6639,10 +6640,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6680,21 +6681,21 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" t="s">
         <v>134</v>
-      </c>
-      <c r="C5" t="s">
-        <v>180</v>
-      </c>
-      <c r="D5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6732,21 +6733,21 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6784,21 +6785,21 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -6836,21 +6837,21 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -6888,21 +6889,21 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -6940,21 +6941,21 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -6992,21 +6993,21 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -7044,21 +7045,21 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -7096,21 +7097,21 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -7148,21 +7149,21 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C59" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -7200,21 +7201,21 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C65" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B67" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -7252,21 +7253,21 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C71" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D71" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B73" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -7304,21 +7305,21 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C77" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D77" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B79" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -7356,21 +7357,21 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D83" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B85" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -7408,21 +7409,21 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C89" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D89" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B91" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -7460,21 +7461,21 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C95" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D95" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B97" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -7512,21 +7513,21 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C101" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D101" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B103" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -7564,21 +7565,21 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C107" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D107" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B109" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -7616,13 +7617,13 @@
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C113" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D113" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -7643,10 +7644,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -7693,24 +7694,24 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" t="s">
         <v>134</v>
-      </c>
-      <c r="C5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D5" t="s">
-        <v>206</v>
-      </c>
-      <c r="E5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -7757,24 +7758,24 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11" t="s">
         <v>208</v>
       </c>
-      <c r="D11" t="s">
-        <v>209</v>
-      </c>
       <c r="E11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -7821,24 +7822,24 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" t="s">
         <v>211</v>
       </c>
-      <c r="D17" t="s">
-        <v>212</v>
-      </c>
       <c r="E17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -7885,24 +7886,24 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -7949,24 +7950,24 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -8013,24 +8014,24 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -8077,24 +8078,24 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -8141,24 +8142,24 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C47" t="s">
+        <v>222</v>
+      </c>
+      <c r="D47" t="s">
         <v>223</v>
       </c>
-      <c r="D47" t="s">
-        <v>224</v>
-      </c>
       <c r="E47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B49" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -8205,24 +8206,24 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C53" t="s">
+        <v>225</v>
+      </c>
+      <c r="D53" t="s">
         <v>226</v>
       </c>
-      <c r="D53" t="s">
-        <v>227</v>
-      </c>
       <c r="E53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -8269,24 +8270,24 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C59" t="s">
+        <v>228</v>
+      </c>
+      <c r="D59" t="s">
         <v>229</v>
       </c>
-      <c r="D59" t="s">
-        <v>230</v>
-      </c>
       <c r="E59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B61" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -8333,24 +8334,24 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C65" t="s">
+        <v>231</v>
+      </c>
+      <c r="D65" t="s">
         <v>232</v>
       </c>
-      <c r="D65" t="s">
-        <v>233</v>
-      </c>
       <c r="E65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -8397,24 +8398,24 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C71" t="s">
+        <v>235</v>
+      </c>
+      <c r="D71" t="s">
         <v>236</v>
       </c>
-      <c r="D71" t="s">
-        <v>237</v>
-      </c>
       <c r="E71" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B73" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -8461,24 +8462,24 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C77" t="s">
+        <v>238</v>
+      </c>
+      <c r="D77" t="s">
         <v>239</v>
       </c>
-      <c r="D77" t="s">
-        <v>240</v>
-      </c>
       <c r="E77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B79" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -8525,16 +8526,16 @@
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C83" t="s">
+        <v>241</v>
+      </c>
+      <c r="D83" t="s">
         <v>242</v>
       </c>
-      <c r="D83" t="s">
-        <v>243</v>
-      </c>
       <c r="E83" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -8555,10 +8556,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -8614,27 +8615,27 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" t="s">
+        <v>246</v>
+      </c>
+      <c r="F5" t="s">
         <v>134</v>
-      </c>
-      <c r="C5" t="s">
-        <v>246</v>
-      </c>
-      <c r="D5" t="s">
-        <v>180</v>
-      </c>
-      <c r="E5" t="s">
-        <v>247</v>
-      </c>
-      <c r="F5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -8690,27 +8691,27 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" t="s">
         <v>249</v>
       </c>
-      <c r="D11" t="s">
-        <v>180</v>
-      </c>
-      <c r="E11" t="s">
-        <v>250</v>
-      </c>
       <c r="F11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -8766,27 +8767,27 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D17" t="s">
+        <v>179</v>
+      </c>
+      <c r="E17" t="s">
         <v>249</v>
       </c>
-      <c r="D17" t="s">
-        <v>180</v>
-      </c>
-      <c r="E17" t="s">
-        <v>250</v>
-      </c>
       <c r="F17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -8842,27 +8843,27 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s">
+        <v>252</v>
+      </c>
+      <c r="D23" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" t="s">
         <v>253</v>
       </c>
-      <c r="D23" t="s">
-        <v>194</v>
-      </c>
-      <c r="E23" t="s">
-        <v>254</v>
-      </c>
       <c r="F23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -8918,27 +8919,27 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E29" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -8994,27 +8995,27 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C35" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D35" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -9070,27 +9071,27 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C41" t="s">
+        <v>262</v>
+      </c>
+      <c r="D41" t="s">
         <v>263</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>264</v>
       </c>
-      <c r="E41" t="s">
-        <v>265</v>
-      </c>
       <c r="F41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -9146,27 +9147,27 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C47" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D47" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E47" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B49" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -9222,27 +9223,27 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C53" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D53" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E53" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -9298,19 +9299,19 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C59" t="s">
+        <v>271</v>
+      </c>
+      <c r="D59" t="s">
+        <v>237</v>
+      </c>
+      <c r="E59" t="s">
         <v>272</v>
       </c>
-      <c r="D59" t="s">
-        <v>238</v>
-      </c>
-      <c r="E59" t="s">
-        <v>273</v>
-      </c>
       <c r="F59" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>